<commit_message>
mejoras en el codigo y chart nuevo
</commit_message>
<xml_diff>
--- a/NMAPP V2.0/app/resources/data.xlsx
+++ b/NMAPP V2.0/app/resources/data.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet name="appear" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="lost" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Stay" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +18,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +60,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -478,4 +484,978 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>hostname</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>port</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>service</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>cve_str</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>dnsmasq</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CVE-2020-25682	8.3	https://vulners.com/cve/CVE-2020-25682;CVE-2020-25681	8.3	https://vulners.com/cve/CVE-2020-25681;CVE-2020-25687	7.1	https://vulners.com/cve/CVE-2020-25687;CVE-2020-25683	7.1	https://vulners.com/cve/CVE-2020-25683;CVE-2017-15107	5.0	https://vulners.com/cve/CVE-2017-15107;OSV:CVE-2020-25685	4.3	https://vulners.com/osv/OSV:CVE-2020-25685;CVE-2021-3448	4.3	https://vulners.com/cve/CVE-2021-3448;CVE-2020-25686	4.3	https://vulners.com/cve/CVE-2020-25686;CVE-2020-25685	4.3	https://vulners.com/cve/CVE-2020-25685;CVE-2020-25684	4.3	https://vulners.com/cve/CVE-2020-25684;CVE-2019-14834	4.3	https://vulners.com/cve/CVE-2019-14834;OSV:CVE-2021-3448	0.0	https://vulners.com/osv/OSV:CVE-2021-3448;CVE-2023-28450	0.0	https://vulners.com/cve/CVE-2023-28450;CVE-2022-0934	0.0	https://vulners.com/cve/CVE-2022-0934</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45056.7021084675</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>8.8.8.8</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>HTTP server (unknown)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" s="2" t="n">
+        <v>45056.70210855079</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>80.245.2.142</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>portugalete.org</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>dnsmasq</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CVE-2020-25682	8.3	https://vulners.com/cve/CVE-2020-25682;CVE-2020-25681	8.3	https://vulners.com/cve/CVE-2020-25681;CVE-2020-25687	7.1	https://vulners.com/cve/CVE-2020-25687;CVE-2020-25683	7.1	https://vulners.com/cve/CVE-2020-25683;CVE-2017-15107	5.0	https://vulners.com/cve/CVE-2017-15107;OSV:CVE-2020-25685	4.3	https://vulners.com/osv/OSV:CVE-2020-25685;CVE-2021-3448	4.3	https://vulners.com/cve/CVE-2021-3448;CVE-2020-25686	4.3	https://vulners.com/cve/CVE-2020-25686;CVE-2020-25685	4.3	https://vulners.com/cve/CVE-2020-25685;CVE-2020-25684	4.3	https://vulners.com/cve/CVE-2020-25684;CVE-2019-14834	4.3	https://vulners.com/cve/CVE-2019-14834;OSV:CVE-2021-3448	0.0	https://vulners.com/osv/OSV:CVE-2021-3448;CVE-2023-28450	0.0	https://vulners.com/cve/CVE-2023-28450;CVE-2022-0934	0.0	https://vulners.com/cve/CVE-2022-0934</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>45056.70661931881</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>80.245.2.142</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>portugalete.org</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>http</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Microsoft IIS httpd</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" s="2" t="n">
+        <v>45056.70661939125</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>80.245.2.142</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>portugalete.org</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>http</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Microsoft IIS httpd</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" s="2" t="n">
+        <v>45056.70661946083</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>80.245.2.142</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>santurtzi.net</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>8008</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>http</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" s="2" t="n">
+        <v>45056.71174195858</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>192.168.0.1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>dnsmasq</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>CVE-2020-25682	8.3	https://vulners.com/cve/CVE-2020-25682;CVE-2020-25681	8.3	https://vulners.com/cve/CVE-2020-25681;CVE-2020-25687	7.1	https://vulners.com/cve/CVE-2020-25687;CVE-2020-25683	7.1	https://vulners.com/cve/CVE-2020-25683;CVE-2017-15107	5.0	https://vulners.com/cve/CVE-2017-15107;OSV:CVE-2020-25685	4.3	https://vulners.com/osv/OSV:CVE-2020-25685;CVE-2021-3448	4.3	https://vulners.com/cve/CVE-2021-3448;CVE-2020-25686	4.3	https://vulners.com/cve/CVE-2020-25686;CVE-2020-25685	4.3	https://vulners.com/cve/CVE-2020-25685;CVE-2020-25684	4.3	https://vulners.com/cve/CVE-2020-25684;CVE-2019-14834	4.3	https://vulners.com/cve/CVE-2019-14834;OSV:CVE-2021-3448	0.0	https://vulners.com/osv/OSV:CVE-2021-3448;CVE-2023-28450	0.0	https://vulners.com/cve/CVE-2023-28450;CVE-2022-0934	0.0	https://vulners.com/cve/CVE-2022-0934</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>45056.71468764382</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>192.168.0.1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>http</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" s="2" t="n">
+        <v>45056.71468771761</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>192.168.0.1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" s="2" t="n">
+        <v>45056.71468779923</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>192.168.0.11</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>3030</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>arepa-cas</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" s="2" t="n">
+        <v>45056.71810147291</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>212.142.136.20</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>bilbao.eus</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>dnsmasq</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>CVE-2020-25682	8.3	https://vulners.com/cve/CVE-2020-25682;CVE-2020-25681	8.3	https://vulners.com/cve/CVE-2020-25681;CVE-2020-25687	7.1	https://vulners.com/cve/CVE-2020-25687;CVE-2020-25683	7.1	https://vulners.com/cve/CVE-2020-25683;CVE-2017-15107	5.0	https://vulners.com/cve/CVE-2017-15107;OSV:CVE-2020-25685	4.3	https://vulners.com/osv/OSV:CVE-2020-25685;CVE-2021-3448	4.3	https://vulners.com/cve/CVE-2021-3448;CVE-2020-25686	4.3	https://vulners.com/cve/CVE-2020-25686;CVE-2020-25685	4.3	https://vulners.com/cve/CVE-2020-25685;CVE-2020-25684	4.3	https://vulners.com/cve/CVE-2020-25684;CVE-2019-14834	4.3	https://vulners.com/cve/CVE-2019-14834;OSV:CVE-2021-3448	0.0	https://vulners.com/osv/OSV:CVE-2021-3448;CVE-2023-28450	0.0	https://vulners.com/cve/CVE-2023-28450;CVE-2022-0934	0.0	https://vulners.com/cve/CVE-2022-0934</t>
+        </is>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>45056.7307383329</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>212.142.136.20</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>bilbao.eus</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>http</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Bilbao WebServer</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" s="2" t="n">
+        <v>45056.73073841707</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>212.142.136.20</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>bilbao.eus</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>https</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Bilbao WebServer</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" s="2" t="n">
+        <v>45056.73073848592</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>80.245.2.142</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>santurtzi.net</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>cisco-sccp</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" s="2" t="n">
+        <v>45057.27608658544</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>80.245.2.142</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>santurtzi.net</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>5060</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>sip</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" s="2" t="n">
+        <v>45057.27608665857</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>212.142.136.20</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>bilbao.eus</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>cisco-sccp</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" s="2" t="n">
+        <v>45057.27608695528</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>212.142.136.20</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>bilbao.eus</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>5060</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>sip</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" s="2" t="n">
+        <v>45057.27608702943</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>80.245.2.142</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>portugalete.org</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>cisco-sccp</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" s="2" t="n">
+        <v>45057.27608760475</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>80.245.2.142</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>portugalete.org</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>5060</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>sip</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" s="2" t="n">
+        <v>45057.27608769016</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>192.168.0.10</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1080</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>socks5</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" s="2" t="n">
+        <v>45062.60961628095</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>192.168.0.10</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>8888</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>tcpwrapped</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" s="2" t="n">
+        <v>45062.6096163524</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ip</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>hostname</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>port</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>protocol</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>service</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>version</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>cve_str</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ts</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>35.206.71.198</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>deusto.es</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ssh</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>OpenSSH</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>CVE-2020-15778	6.8	https://vulners.com/cve/CVE-2020-15778;CVE-2020-12062	5.0	https://vulners.com/cve/CVE-2020-12062;CVE-2021-28041	4.6	https://vulners.com/cve/CVE-2021-28041;CVE-2021-41617	4.4	https://vulners.com/cve/CVE-2021-41617;CVE-2020-14145	4.3	https://vulners.com/cve/CVE-2020-14145;CVE-2016-20012	4.3	https://vulners.com/cve/CVE-2016-20012;CVE-2021-36368	2.6	https://vulners.com/cve/CVE-2021-36368</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>45056.73073855716</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>35.206.71.198</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>deusto.es</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>domain</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>dnsmasq</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CVE-2020-25682	8.3	https://vulners.com/cve/CVE-2020-25682;CVE-2020-25681	8.3	https://vulners.com/cve/CVE-2020-25681;CVE-2020-25687	7.1	https://vulners.com/cve/CVE-2020-25687;CVE-2020-25683	7.1	https://vulners.com/cve/CVE-2020-25683;CVE-2017-15107	5.0	https://vulners.com/cve/CVE-2017-15107;OSV:CVE-2020-25685	4.3	https://vulners.com/osv/OSV:CVE-2020-25685;CVE-2021-3448	4.3	https://vulners.com/cve/CVE-2021-3448;CVE-2020-25686	4.3	https://vulners.com/cve/CVE-2020-25686;CVE-2020-25685	4.3	https://vulners.com/cve/CVE-2020-25685;CVE-2020-25684	4.3	https://vulners.com/cve/CVE-2020-25684;CVE-2019-14834	4.3	https://vulners.com/cve/CVE-2019-14834;OSV:CVE-2021-3448	0.0	https://vulners.com/osv/OSV:CVE-2021-3448;CVE-2023-28450	0.0	https://vulners.com/cve/CVE-2023-28450;CVE-2022-0934	0.0	https://vulners.com/cve/CVE-2022-0934</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>45056.73073862593</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>35.206.71.198</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>deusto.es</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>http</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>lighttpd</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>CVE-2022-22707	4.3	https://vulners.com/cve/CVE-2022-22707;OSV:CVE-2022-41556	0.0	https://vulners.com/osv/OSV:CVE-2022-41556</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>45056.73073869693</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>35.206.71.198</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>deusto.es</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>tcp</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>http</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>lighttpd</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>CVE-2022-22707	4.3	https://vulners.com/cve/CVE-2022-22707;OSV:CVE-2022-41556	0.0	https://vulners.com/osv/OSV:CVE-2022-41556</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>45056.73073876651</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>